<commit_message>
Updates for Day 11
</commit_message>
<xml_diff>
--- a/resources/Forms/Excel/Big Sheet.xlsx
+++ b/resources/Forms/Excel/Big Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dabaxter/Projects/Footie/FootieTake2/resources/Forms/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dabaxter/Projects/Footie_Take2/FootieTake2/resources/Forms/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DEEDEE-79CE-1A43-9CC5-D1B510DA77C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AF3887-6DE8-DC45-9375-435A07CA7A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1920" windowWidth="26820" windowHeight="14720" tabRatio="800" activeTab="1" xr2:uid="{ACDD4B4B-6B95-D34B-BAB9-FF7DBF2FABF6}"/>
   </bookViews>
@@ -442,7 +442,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -489,6 +489,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -796,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -972,25 +979,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1153,21 +1154,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>203199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>410</xdr:row>
-      <xdr:rowOff>15540</xdr:rowOff>
+      <xdr:colOff>467360</xdr:colOff>
+      <xdr:row>407</xdr:row>
+      <xdr:rowOff>49592</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BFCF757-89E6-65BC-3AF4-64F8F6440AD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEDC032-6B79-6542-62C9-C6F72C35543D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1183,8 +1184,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19507200"/>
-          <a:ext cx="8707120" cy="63820340"/>
+          <a:off x="0" y="19303999"/>
+          <a:ext cx="8656320" cy="63447993"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2834,12 +2835,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A17:D17"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A32:D32"/>
@@ -2847,6 +2842,12 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3844,12 +3845,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -3857,6 +3852,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4839,12 +4840,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -4852,6 +4847,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5844,12 +5845,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -5857,6 +5852,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C76" xr:uid="{912C664E-C133-1E4F-9640-4A25EB9EF25D}">
@@ -6845,12 +6846,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -6858,6 +6853,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{B20B3CE4-DCB9-4E4A-AC39-D9DA073FCC61}">
@@ -6873,7 +6874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E206143-2F21-5044-9E67-05C5CD7127D9}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
@@ -7842,12 +7843,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -7855,6 +7850,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8837,12 +8838,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -8850,6 +8845,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9836,12 +9837,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -9849,6 +9844,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C74" xr:uid="{F68D3FFC-EF79-CC40-8F53-8BF21A5E1341}">
@@ -10840,12 +10841,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -10853,6 +10848,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{11A7353F-6A05-F048-B4B5-2330C623E382}">
@@ -11841,6 +11842,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -11848,12 +11855,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{79F4B324-FC19-7044-8ECD-3029BC735257}">
@@ -11870,9 +11871,9 @@
   <dimension ref="A1:CL125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BS1" sqref="BS1"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11928,7 +11929,7 @@
     <col min="66" max="66" width="2.6640625" style="4" customWidth="1"/>
     <col min="67" max="67" width="3.1640625" style="4" customWidth="1"/>
     <col min="68" max="68" width="12.33203125" style="4" customWidth="1"/>
-    <col min="69" max="69" width="5.6640625" style="77" customWidth="1"/>
+    <col min="69" max="69" width="5.6640625" style="4" customWidth="1"/>
     <col min="72" max="72" width="11.33203125" style="4" customWidth="1"/>
     <col min="73" max="73" width="3.33203125" style="4" customWidth="1"/>
     <col min="74" max="74" width="3.5" style="4" customWidth="1"/>
@@ -12064,7 +12065,7 @@
       <c r="BN1" s="48"/>
       <c r="BO1" s="48"/>
       <c r="BP1" s="48"/>
-      <c r="BQ1" s="71" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="BS1" s="5" t="s">
@@ -12331,7 +12332,7 @@
         <f>'Keith G'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ2" s="72">
+      <c r="BQ2" s="3">
         <f>'Keith G'!E52</f>
         <v>0</v>
       </c>
@@ -12354,7 +12355,7 @@
         <f>'Keith G'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX2" s="3">
+      <c r="BX2" s="71">
         <f>'Keith G'!E58</f>
         <v>0</v>
       </c>
@@ -12614,7 +12615,7 @@
         <f>'Keith G'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ3" s="72">
+      <c r="BQ3" s="3">
         <f>'Keith G'!E53</f>
         <v>2</v>
       </c>
@@ -12635,7 +12636,7 @@
         <f>'Keith G'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX3" s="3">
+      <c r="BX3" s="71">
         <f>'Keith G'!E59</f>
         <v>0</v>
       </c>
@@ -12891,7 +12892,7 @@
         <f>'Keith G'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ4" s="72">
+      <c r="BQ4" s="3">
         <f>'Keith G'!E54</f>
         <v>1</v>
       </c>
@@ -12912,7 +12913,7 @@
         <f>'Keith G'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX4" s="3">
+      <c r="BX4" s="71">
         <f>'Keith G'!E60</f>
         <v>0</v>
       </c>
@@ -13170,7 +13171,7 @@
         <f>'Keith G'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ5" s="72">
+      <c r="BQ5" s="3">
         <f>'Keith G'!E55</f>
         <v>2</v>
       </c>
@@ -13191,7 +13192,7 @@
         <f>'Keith G'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX5" s="3">
+      <c r="BX5" s="71">
         <f>'Keith G'!E61</f>
         <v>0</v>
       </c>
@@ -13463,7 +13464,7 @@
         <f>'Stuart L'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ6" s="73">
+      <c r="BQ6" s="18">
         <f>'Stuart L'!E52</f>
         <v>0</v>
       </c>
@@ -13486,7 +13487,7 @@
         <f>'Stuart L'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX6" s="18">
+      <c r="BX6" s="72">
         <f>'Stuart L'!E58</f>
         <v>0</v>
       </c>
@@ -13746,7 +13747,7 @@
         <f>'Stuart L'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ7" s="73">
+      <c r="BQ7" s="18">
         <f>'Stuart L'!E53</f>
         <v>2</v>
       </c>
@@ -13767,7 +13768,7 @@
         <f>'Stuart L'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX7" s="18">
+      <c r="BX7" s="72">
         <f>'Stuart L'!E59</f>
         <v>0</v>
       </c>
@@ -14025,7 +14026,7 @@
         <f>'Stuart L'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ8" s="73">
+      <c r="BQ8" s="18">
         <f>'Stuart L'!E54</f>
         <v>2</v>
       </c>
@@ -14046,7 +14047,7 @@
         <f>'Stuart L'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX8" s="18">
+      <c r="BX8" s="72">
         <f>'Stuart L'!E60</f>
         <v>0</v>
       </c>
@@ -14302,7 +14303,7 @@
         <f>'Stuart L'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ9" s="73">
+      <c r="BQ9" s="18">
         <f>'Stuart L'!E55</f>
         <v>2</v>
       </c>
@@ -14323,7 +14324,7 @@
         <f>'Stuart L'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX9" s="18">
+      <c r="BX9" s="72">
         <f>'Stuart L'!E61</f>
         <v>0</v>
       </c>
@@ -14595,7 +14596,7 @@
         <f>'Barbara L'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ10" s="73">
+      <c r="BQ10" s="18">
         <f>'Barbara L'!E52</f>
         <v>3</v>
       </c>
@@ -14618,7 +14619,7 @@
         <f>'Barbara L'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX10" s="18">
+      <c r="BX10" s="72">
         <f>'Barbara L'!E58</f>
         <v>0</v>
       </c>
@@ -14880,7 +14881,7 @@
         <f>'Barbara L'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ11" s="73">
+      <c r="BQ11" s="18">
         <f>'Barbara L'!E53</f>
         <v>2</v>
       </c>
@@ -14901,7 +14902,7 @@
         <f>'Barbara L'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX11" s="18">
+      <c r="BX11" s="72">
         <f>'Barbara L'!E59</f>
         <v>0</v>
       </c>
@@ -15157,7 +15158,7 @@
         <f>'Barbara L'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ12" s="73">
+      <c r="BQ12" s="18">
         <f>'Barbara L'!E54</f>
         <v>2</v>
       </c>
@@ -15178,7 +15179,7 @@
         <f>'Barbara L'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX12" s="18">
+      <c r="BX12" s="72">
         <f>'Barbara L'!E60</f>
         <v>0</v>
       </c>
@@ -15434,7 +15435,7 @@
         <f>'Barbara L'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ13" s="73">
+      <c r="BQ13" s="18">
         <f>'Barbara L'!E55</f>
         <v>2</v>
       </c>
@@ -15455,7 +15456,7 @@
         <f>'Barbara L'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX13" s="18">
+      <c r="BX13" s="72">
         <f>'Barbara L'!E61</f>
         <v>0</v>
       </c>
@@ -15729,7 +15730,7 @@
         <f>'Freddie J'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ14" s="72">
+      <c r="BQ14" s="3">
         <f>'Freddie J'!E52</f>
         <v>1</v>
       </c>
@@ -15752,7 +15753,7 @@
         <f>'Freddie J'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX14" s="3">
+      <c r="BX14" s="71">
         <f>'Freddie J'!E58</f>
         <v>0</v>
       </c>
@@ -16012,7 +16013,7 @@
         <f>'Freddie J'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ15" s="72">
+      <c r="BQ15" s="3">
         <f>'Freddie J'!E53</f>
         <v>2</v>
       </c>
@@ -16033,7 +16034,7 @@
         <f>'Freddie J'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX15" s="3">
+      <c r="BX15" s="71">
         <f>'Freddie J'!E59</f>
         <v>0</v>
       </c>
@@ -16289,7 +16290,7 @@
         <f>'Freddie J'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ16" s="72">
+      <c r="BQ16" s="3">
         <f>'Freddie J'!E54</f>
         <v>0</v>
       </c>
@@ -16310,7 +16311,7 @@
         <f>'Freddie J'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX16" s="3">
+      <c r="BX16" s="71">
         <f>'Freddie J'!E60</f>
         <v>0</v>
       </c>
@@ -16568,7 +16569,7 @@
         <f>'Freddie J'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ17" s="72">
+      <c r="BQ17" s="3">
         <f>'Freddie J'!E55</f>
         <v>2</v>
       </c>
@@ -16589,7 +16590,7 @@
         <f>'Freddie J'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX17" s="3">
+      <c r="BX17" s="71">
         <f>'Freddie J'!E61</f>
         <v>0</v>
       </c>
@@ -16861,7 +16862,7 @@
         <f>'Mandy B'!D52</f>
         <v>Senegal</v>
       </c>
-      <c r="BQ18" s="72">
+      <c r="BQ18" s="3">
         <f>'Mandy B'!E52</f>
         <v>3</v>
       </c>
@@ -16884,7 +16885,7 @@
         <f>'Mandy B'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX18" s="3">
+      <c r="BX18" s="71">
         <f>'Mandy B'!E58</f>
         <v>0</v>
       </c>
@@ -17144,7 +17145,7 @@
         <f>'Mandy B'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ19" s="72">
+      <c r="BQ19" s="3">
         <f>'Mandy B'!E53</f>
         <v>3</v>
       </c>
@@ -17165,7 +17166,7 @@
         <f>'Mandy B'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX19" s="3">
+      <c r="BX19" s="71">
         <f>'Mandy B'!E59</f>
         <v>0</v>
       </c>
@@ -17423,7 +17424,7 @@
         <f>'Mandy B'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ20" s="72">
+      <c r="BQ20" s="3">
         <f>'Mandy B'!E54</f>
         <v>2</v>
       </c>
@@ -17444,7 +17445,7 @@
         <f>'Mandy B'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX20" s="3">
+      <c r="BX20" s="71">
         <f>'Mandy B'!E60</f>
         <v>0</v>
       </c>
@@ -17700,7 +17701,7 @@
         <f>'Mandy B'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ21" s="72">
+      <c r="BQ21" s="3">
         <f>'Mandy B'!E55</f>
         <v>2</v>
       </c>
@@ -17721,7 +17722,7 @@
         <f>'Mandy B'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX21" s="3">
+      <c r="BX21" s="71">
         <f>'Mandy B'!E61</f>
         <v>0</v>
       </c>
@@ -17993,7 +17994,7 @@
         <f>'Gabriel B'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ22" s="72">
+      <c r="BQ22" s="3">
         <f>'Gabriel B'!E52</f>
         <v>0</v>
       </c>
@@ -18016,7 +18017,7 @@
         <f>'Gabriel B'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX22" s="3">
+      <c r="BX22" s="71">
         <f>'Gabriel B'!E58</f>
         <v>0</v>
       </c>
@@ -18278,7 +18279,7 @@
         <f>'Gabriel B'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ23" s="72">
+      <c r="BQ23" s="3">
         <f>'Gabriel B'!E53</f>
         <v>2</v>
       </c>
@@ -18299,7 +18300,7 @@
         <f>'Gabriel B'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX23" s="3">
+      <c r="BX23" s="71">
         <f>'Gabriel B'!E59</f>
         <v>0</v>
       </c>
@@ -18555,7 +18556,7 @@
         <f>'Gabriel B'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ24" s="72">
+      <c r="BQ24" s="3">
         <f>'Gabriel B'!E54</f>
         <v>0</v>
       </c>
@@ -18576,7 +18577,7 @@
         <f>'Gabriel B'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX24" s="3">
+      <c r="BX24" s="71">
         <f>'Gabriel B'!E60</f>
         <v>0</v>
       </c>
@@ -18832,7 +18833,7 @@
         <f>'Gabriel B'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ25" s="72">
+      <c r="BQ25" s="3">
         <f>'Gabriel B'!E55</f>
         <v>1</v>
       </c>
@@ -18853,7 +18854,7 @@
         <f>'Gabriel B'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX25" s="3">
+      <c r="BX25" s="71">
         <f>'Gabriel B'!E61</f>
         <v>0</v>
       </c>
@@ -19127,7 +19128,7 @@
         <f>'John B'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ26" s="72">
+      <c r="BQ26" s="3">
         <f>'John B'!E52</f>
         <v>0</v>
       </c>
@@ -19150,7 +19151,7 @@
         <f>'John B'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX26" s="3">
+      <c r="BX26" s="71">
         <f>'John B'!E58</f>
         <v>0</v>
       </c>
@@ -19410,7 +19411,7 @@
         <f>'John B'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ27" s="72">
+      <c r="BQ27" s="3">
         <f>'John B'!E53</f>
         <v>2</v>
       </c>
@@ -19431,7 +19432,7 @@
         <f>'John B'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX27" s="3">
+      <c r="BX27" s="71">
         <f>'John B'!E59</f>
         <v>0</v>
       </c>
@@ -19687,7 +19688,7 @@
         <f>'John B'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ28" s="72">
+      <c r="BQ28" s="3">
         <f>'John B'!E54</f>
         <v>2</v>
       </c>
@@ -19708,7 +19709,7 @@
         <f>'John B'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX28" s="3">
+      <c r="BX28" s="71">
         <f>'John B'!E60</f>
         <v>0</v>
       </c>
@@ -19966,7 +19967,7 @@
         <f>'John B'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ29" s="72">
+      <c r="BQ29" s="3">
         <f>'John B'!E55</f>
         <v>2</v>
       </c>
@@ -19987,7 +19988,7 @@
         <f>'John B'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX29" s="3">
+      <c r="BX29" s="71">
         <f>'John B'!E61</f>
         <v>0</v>
       </c>
@@ -20259,7 +20260,7 @@
         <f>'Dawn G'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ30" s="72">
+      <c r="BQ30" s="3">
         <f>'Dawn G'!E52</f>
         <v>0</v>
       </c>
@@ -20282,7 +20283,7 @@
         <f>'Dawn G'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX30" s="3">
+      <c r="BX30" s="71">
         <f>'Dawn G'!E58</f>
         <v>0</v>
       </c>
@@ -20542,7 +20543,7 @@
         <f>'Dawn G'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ31" s="72">
+      <c r="BQ31" s="3">
         <f>'Dawn G'!E53</f>
         <v>2</v>
       </c>
@@ -20563,7 +20564,7 @@
         <f>'Dawn G'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX31" s="3">
+      <c r="BX31" s="71">
         <f>'Dawn G'!E59</f>
         <v>0</v>
       </c>
@@ -20821,7 +20822,7 @@
         <f>'Dawn G'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ32" s="72">
+      <c r="BQ32" s="3">
         <f>'Dawn G'!E54</f>
         <v>1</v>
       </c>
@@ -20842,7 +20843,7 @@
         <f>'Dawn G'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX32" s="3">
+      <c r="BX32" s="71">
         <f>'Dawn G'!E60</f>
         <v>0</v>
       </c>
@@ -21075,7 +21076,7 @@
         <f>'Dawn G'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ33" s="72">
+      <c r="BQ33" s="3">
         <f>'Dawn G'!E55</f>
         <v>3</v>
       </c>
@@ -21096,7 +21097,7 @@
         <f>'Dawn G'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX33" s="3">
+      <c r="BX33" s="71">
         <f>'Dawn G'!E61</f>
         <v>0</v>
       </c>
@@ -21345,7 +21346,7 @@
         <f>'Robert L'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ34" s="72">
+      <c r="BQ34" s="3">
         <f>'Robert L'!E52</f>
         <v>1</v>
       </c>
@@ -21368,7 +21369,7 @@
         <f>'Robert L'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX34" s="3">
+      <c r="BX34" s="71">
         <f>'Robert L'!E58</f>
         <v>0</v>
       </c>
@@ -21607,7 +21608,7 @@
         <f>'Robert L'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ35" s="72">
+      <c r="BQ35" s="3">
         <f>'Robert L'!E53</f>
         <v>3</v>
       </c>
@@ -21628,7 +21629,7 @@
         <f>'Robert L'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX35" s="3">
+      <c r="BX35" s="71">
         <f>'Robert L'!E59</f>
         <v>0</v>
       </c>
@@ -21861,7 +21862,7 @@
         <f>'Robert L'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ36" s="72">
+      <c r="BQ36" s="3">
         <f>'Robert L'!E54</f>
         <v>1</v>
       </c>
@@ -21882,7 +21883,7 @@
         <f>'Robert L'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX36" s="3">
+      <c r="BX36" s="71">
         <f>'Robert L'!E60</f>
         <v>0</v>
       </c>
@@ -22115,7 +22116,7 @@
         <f>'Robert L'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ37" s="72">
+      <c r="BQ37" s="3">
         <f>'Robert L'!E55</f>
         <v>1</v>
       </c>
@@ -22136,7 +22137,7 @@
         <f>'Robert L'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX37" s="3">
+      <c r="BX37" s="71">
         <f>'Robert L'!E61</f>
         <v>0</v>
       </c>
@@ -22387,7 +22388,7 @@
         <f>'Jacques Chi'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ38" s="72">
+      <c r="BQ38" s="3">
         <f>'Jacques Chi'!E52</f>
         <v>0</v>
       </c>
@@ -22410,7 +22411,7 @@
         <f>'Jacques Chi'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX38" s="3">
+      <c r="BX38" s="71">
         <f>'Jacques Chi'!E58</f>
         <v>0</v>
       </c>
@@ -22647,7 +22648,7 @@
         <f>'Jacques Chi'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ39" s="72">
+      <c r="BQ39" s="3">
         <f>'Jacques Chi'!E53</f>
         <v>3</v>
       </c>
@@ -22668,7 +22669,7 @@
         <f>'Jacques Chi'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX39" s="3">
+      <c r="BX39" s="71">
         <f>'Jacques Chi'!E59</f>
         <v>0</v>
       </c>
@@ -22901,7 +22902,7 @@
         <f>'Jacques Chi'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ40" s="72">
+      <c r="BQ40" s="3">
         <f>'Jacques Chi'!E54</f>
         <v>0</v>
       </c>
@@ -22922,7 +22923,7 @@
         <f>'Jacques Chi'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX40" s="3">
+      <c r="BX40" s="71">
         <f>'Jacques Chi'!E60</f>
         <v>0</v>
       </c>
@@ -23157,7 +23158,7 @@
         <f>'Jacques Chi'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ41" s="72">
+      <c r="BQ41" s="3">
         <f>'Jacques Chi'!E55</f>
         <v>2</v>
       </c>
@@ -23178,7 +23179,7 @@
         <f>'Jacques Chi'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX41" s="3">
+      <c r="BX41" s="71">
         <f>'Jacques Chi'!E61</f>
         <v>0</v>
       </c>
@@ -23427,7 +23428,7 @@
         <f>'Dave B'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ42" s="72">
+      <c r="BQ42" s="3">
         <f>'Dave B'!E52</f>
         <v>3</v>
       </c>
@@ -23450,7 +23451,7 @@
         <f>'Dave B'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX42" s="3">
+      <c r="BX42" s="71">
         <f>'Dave B'!E58</f>
         <v>0</v>
       </c>
@@ -23687,7 +23688,7 @@
         <f>'Dave B'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ43" s="72">
+      <c r="BQ43" s="3">
         <f>'Dave B'!E53</f>
         <v>3</v>
       </c>
@@ -23708,7 +23709,7 @@
         <f>'Dave B'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX43" s="3">
+      <c r="BX43" s="71">
         <f>'Dave B'!E59</f>
         <v>0</v>
       </c>
@@ -23943,7 +23944,7 @@
         <f>'Dave B'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ44" s="72">
+      <c r="BQ44" s="3">
         <f>'Dave B'!E54</f>
         <v>1</v>
       </c>
@@ -23964,7 +23965,7 @@
         <f>'Dave B'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX44" s="3">
+      <c r="BX44" s="71">
         <f>'Dave B'!E60</f>
         <v>0</v>
       </c>
@@ -24197,7 +24198,7 @@
         <f>'Dave B'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ45" s="72">
+      <c r="BQ45" s="3">
         <f>'Dave B'!E55</f>
         <v>3</v>
       </c>
@@ -24218,7 +24219,7 @@
         <f>'Dave B'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX45" s="3">
+      <c r="BX45" s="71">
         <f>'Dave B'!E61</f>
         <v>0</v>
       </c>
@@ -24467,7 +24468,7 @@
         <f>'Annaka G-S'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ46" s="72">
+      <c r="BQ46" s="3">
         <f>'Annaka G-S'!E52</f>
         <v>0</v>
       </c>
@@ -24490,7 +24491,7 @@
         <f>'Annaka G-S'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX46" s="3">
+      <c r="BX46" s="71">
         <f>'Annaka G-S'!E58</f>
         <v>0</v>
       </c>
@@ -24729,7 +24730,7 @@
         <f>'Annaka G-S'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ47" s="72">
+      <c r="BQ47" s="3">
         <f>'Annaka G-S'!E53</f>
         <v>0</v>
       </c>
@@ -24750,7 +24751,7 @@
         <f>'Annaka G-S'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX47" s="3">
+      <c r="BX47" s="71">
         <f>'Annaka G-S'!E59</f>
         <v>0</v>
       </c>
@@ -24983,7 +24984,7 @@
         <f>'Annaka G-S'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ48" s="72">
+      <c r="BQ48" s="3">
         <f>'Annaka G-S'!E54</f>
         <v>1</v>
       </c>
@@ -25004,7 +25005,7 @@
         <f>'Annaka G-S'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX48" s="3">
+      <c r="BX48" s="71">
         <f>'Annaka G-S'!E60</f>
         <v>0</v>
       </c>
@@ -25237,7 +25238,7 @@
         <f>'Annaka G-S'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ49" s="72">
+      <c r="BQ49" s="3">
         <f>'Annaka G-S'!E55</f>
         <v>0</v>
       </c>
@@ -25258,7 +25259,7 @@
         <f>'Annaka G-S'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX49" s="3">
+      <c r="BX49" s="71">
         <f>'Annaka G-S'!E61</f>
         <v>0</v>
       </c>
@@ -25509,7 +25510,7 @@
         <f>Claire!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ50" s="72">
+      <c r="BQ50" s="3">
         <f>Claire!E52</f>
         <v>0</v>
       </c>
@@ -25532,7 +25533,7 @@
         <f>Claire!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX50" s="3">
+      <c r="BX50" s="71">
         <f>Claire!E58</f>
         <v>0</v>
       </c>
@@ -25769,7 +25770,7 @@
         <f>Claire!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ51" s="72">
+      <c r="BQ51" s="3">
         <f>Claire!E53</f>
         <v>3</v>
       </c>
@@ -25790,7 +25791,7 @@
         <f>Claire!D59</f>
         <v>France</v>
       </c>
-      <c r="BX51" s="3">
+      <c r="BX51" s="71">
         <f>Claire!E59</f>
         <v>0</v>
       </c>
@@ -26023,7 +26024,7 @@
         <f>Claire!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ52" s="72">
+      <c r="BQ52" s="3">
         <f>Claire!E54</f>
         <v>2</v>
       </c>
@@ -26044,7 +26045,7 @@
         <f>Claire!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX52" s="3">
+      <c r="BX52" s="71">
         <f>Claire!E60</f>
         <v>0</v>
       </c>
@@ -26279,7 +26280,7 @@
         <f>Claire!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ53" s="72">
+      <c r="BQ53" s="3">
         <f>Claire!E55</f>
         <v>0</v>
       </c>
@@ -26300,7 +26301,7 @@
         <f>Claire!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX53" s="3">
+      <c r="BX53" s="71">
         <f>Claire!E61</f>
         <v>0</v>
       </c>
@@ -26549,7 +26550,7 @@
         <f>Hino!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ54" s="72">
+      <c r="BQ54" s="3">
         <f>Hino!E52</f>
         <v>0</v>
       </c>
@@ -26572,7 +26573,7 @@
         <f>Hino!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX54" s="3">
+      <c r="BX54" s="71">
         <f>Hino!E58</f>
         <v>0</v>
       </c>
@@ -26809,7 +26810,7 @@
         <f>Hino!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ55" s="72">
+      <c r="BQ55" s="3">
         <f>Hino!E53</f>
         <v>3</v>
       </c>
@@ -26830,7 +26831,7 @@
         <f>Hino!D59</f>
         <v>France</v>
       </c>
-      <c r="BX55" s="3">
+      <c r="BX55" s="71">
         <f>Hino!E59</f>
         <v>0</v>
       </c>
@@ -27065,7 +27066,7 @@
         <f>Hino!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ56" s="72">
+      <c r="BQ56" s="3">
         <f>Hino!E54</f>
         <v>2</v>
       </c>
@@ -27086,7 +27087,7 @@
         <f>Hino!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX56" s="3">
+      <c r="BX56" s="71">
         <f>Hino!E60</f>
         <v>0</v>
       </c>
@@ -27319,7 +27320,7 @@
         <f>Hino!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ57" s="72">
+      <c r="BQ57" s="3">
         <f>Hino!E55</f>
         <v>2</v>
       </c>
@@ -27340,7 +27341,7 @@
         <f>Hino!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX57" s="3">
+      <c r="BX57" s="71">
         <f>Hino!E61</f>
         <v>0</v>
       </c>
@@ -27589,7 +27590,7 @@
         <f>'Cathy G'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ58" s="72">
+      <c r="BQ58" s="3">
         <f>'Cathy G'!E52</f>
         <v>0</v>
       </c>
@@ -27612,7 +27613,7 @@
         <f>'Cathy G'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX58" s="3">
+      <c r="BX58" s="71">
         <f>'Cathy G'!E58</f>
         <v>0</v>
       </c>
@@ -27851,7 +27852,7 @@
         <f>'Cathy G'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ59" s="72">
+      <c r="BQ59" s="3">
         <f>'Cathy G'!E53</f>
         <v>3</v>
       </c>
@@ -27872,7 +27873,7 @@
         <f>'Cathy G'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX59" s="3">
+      <c r="BX59" s="71">
         <f>'Cathy G'!E59</f>
         <v>0</v>
       </c>
@@ -28105,7 +28106,7 @@
         <f>'Cathy G'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ60" s="72">
+      <c r="BQ60" s="3">
         <f>'Cathy G'!E54</f>
         <v>2</v>
       </c>
@@ -28126,7 +28127,7 @@
         <f>'Cathy G'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX60" s="3">
+      <c r="BX60" s="71">
         <f>'Cathy G'!E60</f>
         <v>0</v>
       </c>
@@ -28359,7 +28360,7 @@
         <f>'Cathy G'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ61" s="72">
+      <c r="BQ61" s="3">
         <f>'Cathy G'!E55</f>
         <v>2</v>
       </c>
@@ -28380,7 +28381,7 @@
         <f>'Cathy G'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX61" s="3">
+      <c r="BX61" s="71">
         <f>'Cathy G'!E61</f>
         <v>0</v>
       </c>
@@ -28631,7 +28632,7 @@
         <f>'Arthur T'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ62" s="72">
+      <c r="BQ62" s="3">
         <f>'Arthur T'!E52</f>
         <v>0</v>
       </c>
@@ -28654,7 +28655,7 @@
         <f>'Arthur T'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX62" s="3">
+      <c r="BX62" s="71">
         <f>'Arthur T'!E58</f>
         <v>0</v>
       </c>
@@ -28891,7 +28892,7 @@
         <f>'Arthur T'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ63" s="72">
+      <c r="BQ63" s="3">
         <f>'Arthur T'!E53</f>
         <v>3</v>
       </c>
@@ -28912,7 +28913,7 @@
         <f>'Arthur T'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX63" s="3">
+      <c r="BX63" s="71">
         <f>'Arthur T'!E59</f>
         <v>0</v>
       </c>
@@ -29145,7 +29146,7 @@
         <f>'Arthur T'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ64" s="72">
+      <c r="BQ64" s="3">
         <f>'Arthur T'!E54</f>
         <v>1</v>
       </c>
@@ -29166,7 +29167,7 @@
         <f>'Arthur T'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX64" s="3">
+      <c r="BX64" s="71">
         <f>'Arthur T'!E60</f>
         <v>0</v>
       </c>
@@ -29401,7 +29402,7 @@
         <f>'Arthur T'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ65" s="72">
+      <c r="BQ65" s="3">
         <f>'Arthur T'!E55</f>
         <v>0</v>
       </c>
@@ -29422,7 +29423,7 @@
         <f>'Arthur T'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX65" s="3">
+      <c r="BX65" s="71">
         <f>'Arthur T'!E61</f>
         <v>0</v>
       </c>
@@ -29671,7 +29672,7 @@
         <f>'Andy B'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ66" s="72">
+      <c r="BQ66" s="3">
         <f>'Andy B'!E52</f>
         <v>0</v>
       </c>
@@ -29694,7 +29695,7 @@
         <f>'Andy B'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX66" s="3">
+      <c r="BX66" s="71">
         <f>'Andy B'!E58</f>
         <v>0</v>
       </c>
@@ -29931,7 +29932,7 @@
         <f>'Andy B'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ67" s="72">
+      <c r="BQ67" s="3">
         <f>'Andy B'!E53</f>
         <v>2</v>
       </c>
@@ -29952,7 +29953,7 @@
         <f>'Andy B'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX67" s="3">
+      <c r="BX67" s="71">
         <f>'Andy B'!E59</f>
         <v>0</v>
       </c>
@@ -30187,7 +30188,7 @@
         <f>'Andy B'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ68" s="72">
+      <c r="BQ68" s="3">
         <f>'Andy B'!E54</f>
         <v>1</v>
       </c>
@@ -30208,7 +30209,7 @@
         <f>'Andy B'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX68" s="3">
+      <c r="BX68" s="71">
         <f>'Andy B'!E60</f>
         <v>0</v>
       </c>
@@ -30441,7 +30442,7 @@
         <f>'Andy B'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ69" s="72">
+      <c r="BQ69" s="3">
         <f>'Andy B'!E55</f>
         <v>1</v>
       </c>
@@ -30462,7 +30463,7 @@
         <f>'Andy B'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX69" s="3">
+      <c r="BX69" s="71">
         <f>'Andy B'!E61</f>
         <v>0</v>
       </c>
@@ -30711,7 +30712,7 @@
         <f>'Alison S'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ70" s="74">
+      <c r="BQ70" s="34">
         <f>'Alison S'!E52</f>
         <v>0</v>
       </c>
@@ -30734,7 +30735,7 @@
         <f>'Alison S'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX70" s="34">
+      <c r="BX70" s="73">
         <f>'Alison S'!E58</f>
         <v>0</v>
       </c>
@@ -30973,7 +30974,7 @@
         <f>'Alison S'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ71" s="74">
+      <c r="BQ71" s="34">
         <f>'Alison S'!E53</f>
         <v>3</v>
       </c>
@@ -30994,7 +30995,7 @@
         <f>'Alison S'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX71" s="34">
+      <c r="BX71" s="73">
         <f>'Alison S'!E59</f>
         <v>0</v>
       </c>
@@ -31227,7 +31228,7 @@
         <f>'Alison S'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ72" s="74">
+      <c r="BQ72" s="34">
         <f>'Alison S'!E54</f>
         <v>2</v>
       </c>
@@ -31248,7 +31249,7 @@
         <f>'Alison S'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX72" s="34">
+      <c r="BX72" s="73">
         <f>'Alison S'!E60</f>
         <v>0</v>
       </c>
@@ -31481,7 +31482,7 @@
         <f>'Alison S'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ73" s="74">
+      <c r="BQ73" s="34">
         <f>'Alison S'!E55</f>
         <v>3</v>
       </c>
@@ -31502,7 +31503,7 @@
         <f>'Alison S'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX73" s="34">
+      <c r="BX73" s="73">
         <f>'Alison S'!E61</f>
         <v>0</v>
       </c>
@@ -31753,7 +31754,7 @@
         <f>'Evan A'!D52</f>
         <v>Senegal</v>
       </c>
-      <c r="BQ74" s="74">
+      <c r="BQ74" s="34">
         <f>'Evan A'!E52</f>
         <v>0</v>
       </c>
@@ -31776,7 +31777,7 @@
         <f>'Evan A'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX74" s="34">
+      <c r="BX74" s="73">
         <f>'Evan A'!E58</f>
         <v>0</v>
       </c>
@@ -32013,7 +32014,7 @@
         <f>'Evan A'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ75" s="74">
+      <c r="BQ75" s="34">
         <f>'Evan A'!E53</f>
         <v>3</v>
       </c>
@@ -32034,7 +32035,7 @@
         <f>'Evan A'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX75" s="34">
+      <c r="BX75" s="73">
         <f>'Evan A'!E59</f>
         <v>0</v>
       </c>
@@ -32267,7 +32268,7 @@
         <f>'Evan A'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ76" s="74">
+      <c r="BQ76" s="34">
         <f>'Evan A'!E54</f>
         <v>2</v>
       </c>
@@ -32288,7 +32289,7 @@
         <f>'Evan A'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX76" s="34">
+      <c r="BX76" s="73">
         <f>'Evan A'!E60</f>
         <v>0</v>
       </c>
@@ -32523,7 +32524,7 @@
         <f>'Evan A'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ77" s="74">
+      <c r="BQ77" s="34">
         <f>'Evan A'!E55</f>
         <v>1</v>
       </c>
@@ -32544,7 +32545,7 @@
         <f>'Evan A'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX77" s="34">
+      <c r="BX77" s="73">
         <f>'Evan A'!E61</f>
         <v>0</v>
       </c>
@@ -32793,7 +32794,7 @@
         <f>'Rob TH'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ78" s="74">
+      <c r="BQ78" s="34">
         <f>'Rob TH'!E52</f>
         <v>3</v>
       </c>
@@ -32816,7 +32817,7 @@
         <f>'Rob TH'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX78" s="34">
+      <c r="BX78" s="73">
         <f>'Rob TH'!E58</f>
         <v>0</v>
       </c>
@@ -33053,7 +33054,7 @@
         <f>'Rob TH'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ79" s="74">
+      <c r="BQ79" s="34">
         <f>'Rob TH'!E53</f>
         <v>2</v>
       </c>
@@ -33074,7 +33075,7 @@
         <f>'Rob TH'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX79" s="34">
+      <c r="BX79" s="73">
         <f>'Rob TH'!E59</f>
         <v>0</v>
       </c>
@@ -33309,7 +33310,7 @@
         <f>'Rob TH'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ80" s="74">
+      <c r="BQ80" s="34">
         <f>'Rob TH'!E54</f>
         <v>2</v>
       </c>
@@ -33330,7 +33331,7 @@
         <f>'Rob TH'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX80" s="34">
+      <c r="BX80" s="73">
         <f>'Rob TH'!E60</f>
         <v>0</v>
       </c>
@@ -33563,7 +33564,7 @@
         <f>'Rob TH'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ81" s="74">
+      <c r="BQ81" s="34">
         <f>'Rob TH'!E55</f>
         <v>2</v>
       </c>
@@ -33584,7 +33585,7 @@
         <f>'Rob TH'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX81" s="34">
+      <c r="BX81" s="73">
         <f>'Rob TH'!E61</f>
         <v>0</v>
       </c>
@@ -33833,7 +33834,7 @@
         <f>'Alice D'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ82" s="74">
+      <c r="BQ82" s="34">
         <f>'Alice D'!E52</f>
         <v>0</v>
       </c>
@@ -33856,7 +33857,7 @@
         <f>'Alice D'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX82" s="34">
+      <c r="BX82" s="73">
         <f>'Alice D'!E58</f>
         <v>0</v>
       </c>
@@ -34095,7 +34096,7 @@
         <f>'Alice D'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ83" s="74">
+      <c r="BQ83" s="34">
         <f>'Alice D'!E53</f>
         <v>3</v>
       </c>
@@ -34116,7 +34117,7 @@
         <f>'Alice D'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX83" s="34">
+      <c r="BX83" s="73">
         <f>'Alice D'!E59</f>
         <v>0</v>
       </c>
@@ -34349,7 +34350,7 @@
         <f>'Alice D'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ84" s="74">
+      <c r="BQ84" s="34">
         <f>'Alice D'!E54</f>
         <v>2</v>
       </c>
@@ -34370,7 +34371,7 @@
         <f>'Alice D'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX84" s="34">
+      <c r="BX84" s="73">
         <f>'Alice D'!E60</f>
         <v>0</v>
       </c>
@@ -34603,7 +34604,7 @@
         <f>'Alice D'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ85" s="74">
+      <c r="BQ85" s="34">
         <f>'Alice D'!E55</f>
         <v>0</v>
       </c>
@@ -34624,7 +34625,7 @@
         <f>'Alice D'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX85" s="34">
+      <c r="BX85" s="73">
         <f>'Alice D'!E61</f>
         <v>0</v>
       </c>
@@ -34875,7 +34876,7 @@
         <f>'Liz W'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ86" s="74">
+      <c r="BQ86" s="34">
         <f>'Liz W'!E52</f>
         <v>0</v>
       </c>
@@ -34898,7 +34899,7 @@
         <f>'Liz W'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX86" s="34">
+      <c r="BX86" s="73">
         <f>'Liz W'!E58</f>
         <v>0</v>
       </c>
@@ -35135,7 +35136,7 @@
         <f>'Liz W'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ87" s="74">
+      <c r="BQ87" s="34">
         <f>'Liz W'!E53</f>
         <v>3</v>
       </c>
@@ -35156,7 +35157,7 @@
         <f>'Liz W'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX87" s="34">
+      <c r="BX87" s="73">
         <f>'Liz W'!E59</f>
         <v>0</v>
       </c>
@@ -35389,7 +35390,7 @@
         <f>'Liz W'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ88" s="74">
+      <c r="BQ88" s="34">
         <f>'Liz W'!E54</f>
         <v>1</v>
       </c>
@@ -35410,7 +35411,7 @@
         <f>'Liz W'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX88" s="34">
+      <c r="BX88" s="73">
         <f>'Liz W'!E60</f>
         <v>0</v>
       </c>
@@ -35645,7 +35646,7 @@
         <f>'Liz W'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ89" s="74">
+      <c r="BQ89" s="34">
         <f>'Liz W'!E55</f>
         <v>2</v>
       </c>
@@ -35666,7 +35667,7 @@
         <f>'Liz W'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX89" s="34">
+      <c r="BX89" s="73">
         <f>'Liz W'!E61</f>
         <v>0</v>
       </c>
@@ -35915,7 +35916,7 @@
         <f>'Keith W'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ90" s="74">
+      <c r="BQ90" s="34">
         <f>'Keith W'!E52</f>
         <v>3</v>
       </c>
@@ -35938,7 +35939,7 @@
         <f>'Keith W'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX90" s="34">
+      <c r="BX90" s="73">
         <f>'Keith W'!E58</f>
         <v>0</v>
       </c>
@@ -36175,7 +36176,7 @@
         <f>'Keith W'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ91" s="74">
+      <c r="BQ91" s="34">
         <f>'Keith W'!E53</f>
         <v>2</v>
       </c>
@@ -36196,7 +36197,7 @@
         <f>'Keith W'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX91" s="34">
+      <c r="BX91" s="73">
         <f>'Keith W'!E59</f>
         <v>0</v>
       </c>
@@ -36431,7 +36432,7 @@
         <f>'Keith W'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ92" s="74">
+      <c r="BQ92" s="34">
         <f>'Keith W'!E54</f>
         <v>2</v>
       </c>
@@ -36452,7 +36453,7 @@
         <f>'Keith W'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX92" s="34">
+      <c r="BX92" s="73">
         <f>'Keith W'!E60</f>
         <v>0</v>
       </c>
@@ -36685,7 +36686,7 @@
         <f>'Keith W'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ93" s="74">
+      <c r="BQ93" s="34">
         <f>'Keith W'!E55</f>
         <v>2</v>
       </c>
@@ -36706,7 +36707,7 @@
         <f>'Keith W'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX93" s="34">
+      <c r="BX93" s="73">
         <f>'Keith W'!E61</f>
         <v>0</v>
       </c>
@@ -36955,7 +36956,7 @@
         <f>'Marjorie L'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ94" s="75">
+      <c r="BQ94" s="36">
         <f>'Marjorie L'!E52</f>
         <v>0</v>
       </c>
@@ -36978,7 +36979,7 @@
         <f>'Marjorie L'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX94" s="36">
+      <c r="BX94" s="74">
         <f>'Marjorie L'!E58</f>
         <v>0</v>
       </c>
@@ -37194,7 +37195,7 @@
         <f>'Marjorie L'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ95" s="75">
+      <c r="BQ95" s="36">
         <f>'Marjorie L'!E53</f>
         <v>2</v>
       </c>
@@ -37215,7 +37216,7 @@
         <f>'Marjorie L'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX95" s="36">
+      <c r="BX95" s="74">
         <f>'Marjorie L'!E59</f>
         <v>0</v>
       </c>
@@ -37427,7 +37428,7 @@
         <f>'Marjorie L'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ96" s="75">
+      <c r="BQ96" s="36">
         <f>'Marjorie L'!E54</f>
         <v>1</v>
       </c>
@@ -37448,7 +37449,7 @@
         <f>'Marjorie L'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX96" s="36">
+      <c r="BX96" s="74">
         <f>'Marjorie L'!E60</f>
         <v>0</v>
       </c>
@@ -37660,7 +37661,7 @@
         <f>'Marjorie L'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ97" s="75">
+      <c r="BQ97" s="36">
         <f>'Marjorie L'!E55</f>
         <v>0</v>
       </c>
@@ -37681,7 +37682,7 @@
         <f>'Marjorie L'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX97" s="36">
+      <c r="BX97" s="74">
         <f>'Marjorie L'!E61</f>
         <v>0</v>
       </c>
@@ -37909,7 +37910,7 @@
         <f>'Martin L'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ98" s="75">
+      <c r="BQ98" s="36">
         <f>'Martin L'!E52</f>
         <v>0</v>
       </c>
@@ -37932,7 +37933,7 @@
         <f>'Martin L'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX98" s="36">
+      <c r="BX98" s="74">
         <f>'Martin L'!E58</f>
         <v>0</v>
       </c>
@@ -38148,7 +38149,7 @@
         <f>'Martin L'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ99" s="75">
+      <c r="BQ99" s="36">
         <f>'Martin L'!E53</f>
         <v>1</v>
       </c>
@@ -38169,7 +38170,7 @@
         <f>'Martin L'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX99" s="36">
+      <c r="BX99" s="74">
         <f>'Martin L'!E59</f>
         <v>0</v>
       </c>
@@ -38381,7 +38382,7 @@
         <f>'Martin L'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ100" s="75">
+      <c r="BQ100" s="36">
         <f>'Martin L'!E54</f>
         <v>2</v>
       </c>
@@ -38402,7 +38403,7 @@
         <f>'Martin L'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX100" s="36">
+      <c r="BX100" s="74">
         <f>'Martin L'!E60</f>
         <v>0</v>
       </c>
@@ -38614,7 +38615,7 @@
         <f>'Martin L'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ101" s="75">
+      <c r="BQ101" s="36">
         <f>'Martin L'!E55</f>
         <v>1</v>
       </c>
@@ -38635,7 +38636,7 @@
         <f>'Martin L'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX101" s="36">
+      <c r="BX101" s="74">
         <f>'Martin L'!E61</f>
         <v>0</v>
       </c>
@@ -38863,7 +38864,7 @@
         <f>'Nathan W'!D43</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ102" s="74">
+      <c r="BQ102" s="34">
         <f>'Nathan W'!E43</f>
         <v>3</v>
       </c>
@@ -38886,7 +38887,7 @@
         <f>'Nathan W'!D48</f>
         <v>Denmark</v>
       </c>
-      <c r="BX102" s="34">
+      <c r="BX102" s="73">
         <f>'Nathan W'!E48</f>
         <v>0</v>
       </c>
@@ -39102,7 +39103,7 @@
         <f>'Nathan W'!D44</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ103" s="74">
+      <c r="BQ103" s="34">
         <f>'Nathan W'!E44</f>
         <v>1</v>
       </c>
@@ -39123,7 +39124,7 @@
         <f>'Nathan W'!D49</f>
         <v>France</v>
       </c>
-      <c r="BX103" s="34">
+      <c r="BX103" s="73">
         <f>'Nathan W'!E49</f>
         <v>0</v>
       </c>
@@ -39335,7 +39336,7 @@
         <f>'Nathan W'!D45</f>
         <v>England</v>
       </c>
-      <c r="BQ104" s="74">
+      <c r="BQ104" s="34">
         <f>'Nathan W'!E45</f>
         <v>1</v>
       </c>
@@ -39356,7 +39357,7 @@
         <f>'Nathan W'!D50</f>
         <v>Argentina</v>
       </c>
-      <c r="BX104" s="34">
+      <c r="BX104" s="73">
         <f>'Nathan W'!E50</f>
         <v>0</v>
       </c>
@@ -39568,7 +39569,7 @@
         <f>'Nathan W'!D46</f>
         <v>United States</v>
       </c>
-      <c r="BQ105" s="74">
+      <c r="BQ105" s="34">
         <f>'Nathan W'!E46</f>
         <v>1</v>
       </c>
@@ -39589,7 +39590,7 @@
         <f>'Nathan W'!D51</f>
         <v>Mexico</v>
       </c>
-      <c r="BX105" s="34">
+      <c r="BX105" s="73">
         <f>'Nathan W'!E51</f>
         <v>0</v>
       </c>
@@ -39817,7 +39818,7 @@
         <f>'Bernie R'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ106" s="74">
+      <c r="BQ106" s="34">
         <f>'Bernie R'!E52</f>
         <v>0</v>
       </c>
@@ -39840,7 +39841,7 @@
         <f>'Bernie R'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX106" s="34">
+      <c r="BX106" s="73">
         <f>'Bernie R'!E58</f>
         <v>0</v>
       </c>
@@ -40056,7 +40057,7 @@
         <f>'Bernie R'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ107" s="74">
+      <c r="BQ107" s="34">
         <f>'Bernie R'!E53</f>
         <v>3</v>
       </c>
@@ -40077,7 +40078,7 @@
         <f>'Bernie R'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX107" s="34">
+      <c r="BX107" s="73">
         <f>'Bernie R'!E59</f>
         <v>0</v>
       </c>
@@ -40289,7 +40290,7 @@
         <f>'Bernie R'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ108" s="74">
+      <c r="BQ108" s="34">
         <f>'Bernie R'!E54</f>
         <v>1</v>
       </c>
@@ -40310,7 +40311,7 @@
         <f>'Bernie R'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX108" s="34">
+      <c r="BX108" s="73">
         <f>'Bernie R'!E60</f>
         <v>0</v>
       </c>
@@ -40522,7 +40523,7 @@
         <f>'Bernie R'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ109" s="74">
+      <c r="BQ109" s="34">
         <f>'Bernie R'!E55</f>
         <v>2</v>
       </c>
@@ -40543,7 +40544,7 @@
         <f>'Bernie R'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX109" s="34">
+      <c r="BX109" s="73">
         <f>'Bernie R'!E61</f>
         <v>0</v>
       </c>
@@ -40771,7 +40772,7 @@
         <f>'Derek b'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ110" s="76">
+      <c r="BQ110" s="38">
         <f>'Derek b'!E52</f>
         <v>0</v>
       </c>
@@ -40794,7 +40795,7 @@
         <f>'Derek b'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX110" s="38">
+      <c r="BX110" s="75">
         <f>'Derek b'!E58</f>
         <v>0</v>
       </c>
@@ -41010,7 +41011,7 @@
         <f>'Derek b'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ111" s="76">
+      <c r="BQ111" s="38">
         <f>'Derek b'!E53</f>
         <v>2</v>
       </c>
@@ -41031,7 +41032,7 @@
         <f>'Derek b'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX111" s="38">
+      <c r="BX111" s="75">
         <f>'Derek b'!E59</f>
         <v>0</v>
       </c>
@@ -41243,7 +41244,7 @@
         <f>'Derek b'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ112" s="76">
+      <c r="BQ112" s="38">
         <f>'Derek b'!E54</f>
         <v>1</v>
       </c>
@@ -41264,7 +41265,7 @@
         <f>'Derek b'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX112" s="38">
+      <c r="BX112" s="75">
         <f>'Derek b'!E60</f>
         <v>0</v>
       </c>
@@ -41476,7 +41477,7 @@
         <f>'Derek b'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ113" s="76">
+      <c r="BQ113" s="38">
         <f>'Derek b'!E55</f>
         <v>1</v>
       </c>
@@ -41497,7 +41498,7 @@
         <f>'Derek b'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX113" s="38">
+      <c r="BX113" s="75">
         <f>'Derek b'!E61</f>
         <v>0</v>
       </c>
@@ -41725,7 +41726,7 @@
         <f>'Mother B'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ114" s="76">
+      <c r="BQ114" s="38">
         <f>'Mother B'!E52</f>
         <v>0</v>
       </c>
@@ -41748,7 +41749,7 @@
         <f>'Mother B'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX114" s="38">
+      <c r="BX114" s="75">
         <f>'Mother B'!E58</f>
         <v>0</v>
       </c>
@@ -41964,7 +41965,7 @@
         <f>'Mother B'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ115" s="76">
+      <c r="BQ115" s="38">
         <f>'Mother B'!E53</f>
         <v>1</v>
       </c>
@@ -41985,7 +41986,7 @@
         <f>'Mother B'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX115" s="38">
+      <c r="BX115" s="75">
         <f>'Mother B'!E59</f>
         <v>0</v>
       </c>
@@ -42197,7 +42198,7 @@
         <f>'Mother B'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ116" s="76">
+      <c r="BQ116" s="38">
         <f>'Mother B'!E54</f>
         <v>0</v>
       </c>
@@ -42218,7 +42219,7 @@
         <f>'Mother B'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX116" s="38">
+      <c r="BX116" s="75">
         <f>'Mother B'!E60</f>
         <v>0</v>
       </c>
@@ -42430,7 +42431,7 @@
         <f>'Mother B'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ117" s="76">
+      <c r="BQ117" s="38">
         <f>'Mother B'!E55</f>
         <v>1</v>
       </c>
@@ -42451,7 +42452,7 @@
         <f>'Mother B'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX117" s="38">
+      <c r="BX117" s="75">
         <f>'Mother B'!E61</f>
         <v>0</v>
       </c>
@@ -42679,7 +42680,7 @@
         <f>'James W'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ118" s="76">
+      <c r="BQ118" s="38">
         <f>'James W'!E52</f>
         <v>1</v>
       </c>
@@ -42702,7 +42703,7 @@
         <f>'James W'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX118" s="38">
+      <c r="BX118" s="75">
         <f>'James W'!E58</f>
         <v>0</v>
       </c>
@@ -42918,7 +42919,7 @@
         <f>'James W'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ119" s="76">
+      <c r="BQ119" s="38">
         <f>'James W'!E53</f>
         <v>2</v>
       </c>
@@ -42939,7 +42940,7 @@
         <f>'James W'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX119" s="38">
+      <c r="BX119" s="75">
         <f>'James W'!E59</f>
         <v>0</v>
       </c>
@@ -43151,7 +43152,7 @@
         <f>'James W'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ120" s="76">
+      <c r="BQ120" s="38">
         <f>'James W'!E54</f>
         <v>0</v>
       </c>
@@ -43172,7 +43173,7 @@
         <f>'James W'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX120" s="38">
+      <c r="BX120" s="75">
         <f>'James W'!E60</f>
         <v>0</v>
       </c>
@@ -43384,7 +43385,7 @@
         <f>'James W'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ121" s="76">
+      <c r="BQ121" s="38">
         <f>'James W'!E55</f>
         <v>1</v>
       </c>
@@ -43405,7 +43406,7 @@
         <f>'James W'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX121" s="38">
+      <c r="BX121" s="75">
         <f>'James W'!E61</f>
         <v>0</v>
       </c>
@@ -43633,7 +43634,7 @@
         <f>'Nikki W'!D52</f>
         <v>Sengal</v>
       </c>
-      <c r="BQ122" s="76">
+      <c r="BQ122" s="38">
         <f>'Nikki W'!E52</f>
         <v>0</v>
       </c>
@@ -43656,7 +43657,7 @@
         <f>'Nikki W'!D58</f>
         <v>Denmark</v>
       </c>
-      <c r="BX122" s="38">
+      <c r="BX122" s="75">
         <f>'Nikki W'!E58</f>
         <v>0</v>
       </c>
@@ -43872,7 +43873,7 @@
         <f>'Nikki W'!D53</f>
         <v>Qatar</v>
       </c>
-      <c r="BQ123" s="76">
+      <c r="BQ123" s="38">
         <f>'Nikki W'!E53</f>
         <v>2</v>
       </c>
@@ -43893,7 +43894,7 @@
         <f>'Nikki W'!D59</f>
         <v>France</v>
       </c>
-      <c r="BX123" s="38">
+      <c r="BX123" s="75">
         <f>'Nikki W'!E59</f>
         <v>0</v>
       </c>
@@ -44105,7 +44106,7 @@
         <f>'Nikki W'!D54</f>
         <v>England</v>
       </c>
-      <c r="BQ124" s="76">
+      <c r="BQ124" s="38">
         <f>'Nikki W'!E54</f>
         <v>2</v>
       </c>
@@ -44126,7 +44127,7 @@
         <f>'Nikki W'!D60</f>
         <v>Argentina</v>
       </c>
-      <c r="BX124" s="38">
+      <c r="BX124" s="75">
         <f>'Nikki W'!E60</f>
         <v>0</v>
       </c>
@@ -44338,7 +44339,7 @@
         <f>'Nikki W'!D55</f>
         <v>United States</v>
       </c>
-      <c r="BQ125" s="76">
+      <c r="BQ125" s="38">
         <f>'Nikki W'!E55</f>
         <v>2</v>
       </c>
@@ -44359,7 +44360,7 @@
         <f>'Nikki W'!D61</f>
         <v>Mexico</v>
       </c>
-      <c r="BX125" s="38">
+      <c r="BX125" s="75">
         <f>'Nikki W'!E61</f>
         <v>0</v>
       </c>
@@ -44408,12 +44409,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AK1:AN1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="AR1:AU1"/>
     <mergeCell ref="AY1:BB1"/>
@@ -44421,6 +44416,12 @@
     <mergeCell ref="BM1:BP1"/>
     <mergeCell ref="BT1:BW1"/>
     <mergeCell ref="CA1:CD1"/>
+    <mergeCell ref="AK1:AN1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="AD1:AG1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -45387,12 +45388,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -45400,6 +45395,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49293,12 +49294,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -49306,6 +49301,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67:C73 B66 B1:C65" xr:uid="{156C7248-1706-4E17-9BB6-079B78DEF479}">
@@ -50294,12 +50295,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -50307,6 +50302,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{05F05F3A-89C6-E74F-BB5C-B82EDA718869}">
@@ -51295,12 +51296,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -51308,6 +51303,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{A2199F60-9E4F-6445-90E3-92673D510A9D}">
@@ -52296,6 +52297,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -52303,12 +52310,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{2B53EE05-D1D3-374E-8836-2425C3E2B4A5}">
@@ -53303,6 +53304,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -53310,12 +53317,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C75" xr:uid="{A6BA8386-7538-B943-BC89-6C717665472C}">
@@ -54304,6 +54305,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -54311,12 +54318,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{CBEDE9B1-CCD8-024F-8FF6-52E83D09DD5F}">
@@ -54883,18 +54884,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B22:E22"/>
     <mergeCell ref="B64:E64"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -55877,6 +55878,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -55884,12 +55891,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{9D4EDCA2-2FFE-E64B-A34E-466DD99F6343}">
@@ -56878,6 +56879,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -56885,12 +56892,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -57873,12 +57874,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -57886,6 +57881,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{8427FA4B-D7DC-C74F-B6C6-02A04CEA1479}">
@@ -58877,12 +58878,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -58890,6 +58885,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{8A242A5A-737B-3248-9203-1E18FA7E8CAD}">
@@ -59878,6 +59879,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -59885,12 +59892,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60873,6 +60874,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -60880,12 +60887,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -62094,12 +62095,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -62107,6 +62102,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{98289B19-A16E-8E48-AC84-DA2AC3E66DBF}">
@@ -63095,6 +63096,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -63102,12 +63109,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -64090,12 +64091,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -64103,6 +64098,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{F2D3BCCF-F868-974E-AEC9-AB88E8DBE8B7}">
@@ -65091,12 +65092,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -65104,6 +65099,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{85A9722B-955B-CF41-A6F3-38FDC4B48A7A}">
@@ -66092,12 +66093,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A39:D39"/>
@@ -66105,6 +66100,12 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C73" xr:uid="{A72D56DF-9BC0-2E49-9D2A-B8E721479EEF}">

</xml_diff>